<commit_message>
cambios home y pruebita
</commit_message>
<xml_diff>
--- a/my-chatbot/client/public/Universidades1.xlsx
+++ b/my-chatbot/client/public/Universidades1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martingotz/Desktop/Tesis/Datos /"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B78C5CA-04BD-EE40-ACF1-BD95B27E8E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A83701D-FC88-4499-AE39-25C580191B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{734B2E0E-EC6D-3043-8697-C844BDEEE9AC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{734B2E0E-EC6D-3043-8697-C844BDEEE9AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -106,9 +106,6 @@
     <t>ingreso@uca.edu.ar</t>
   </si>
   <si>
-    <t xml:space="preserve">Instagram </t>
-  </si>
-  <si>
     <t>Twitter</t>
   </si>
   <si>
@@ -166,12 +163,6 @@
     <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcTMhxIAvfGuy1fJP2SbILWDYqDk67O7gLmW1A&amp;s</t>
   </si>
   <si>
-    <t>https://artenlinea.s3-accelerate.amazonaws.com/digital_files/510/large_10177922_808898155804372_6764366353506386933_n.png</t>
-  </si>
-  <si>
-    <t>https://upload.wikimedia.org/wikipedia/commons/4/4c/Bandera-uca.png</t>
-  </si>
-  <si>
     <t>Ranking</t>
   </si>
   <si>
@@ -224,13 +215,22 @@
   </si>
   <si>
     <t>https://www.topuniversities.com/world-university-rankings/2024?tab=indicators&amp;countries=ar&amp;sort_by=rank&amp;order_by=asc</t>
+  </si>
+  <si>
+    <t>Instagram</t>
+  </si>
+  <si>
+    <t>https://www.utdtest.com/Themes2G/comunicaciones/Images/logo-secundario.svg</t>
+  </si>
+  <si>
+    <t>https://scontent.faep24-1.fna.fbcdn.net/v/t39.30808-6/327436997_1930120767319004_2025655574534719690_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=6ee11a&amp;_nc_ohc=ZT5iJ-GczfIQ7kNvgGLXHT7&amp;_nc_ht=scontent.faep24-1.fna&amp;oh=00_AYCs68elqgKBSAsJJ5NhhFSDiMgx3CzdCr7dlHREroTiag&amp;oe=668CB904</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -305,9 +305,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -345,7 +345,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -451,7 +451,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -593,7 +593,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -603,35 +603,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B75DD394-886A-F744-89DD-50EC7F0E0F44}">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="62.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.296875" customWidth="1"/>
+    <col min="3" max="3" width="16.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.69921875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="25.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.69921875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="45" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="79.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="114.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="114.796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="43.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -640,39 +640,39 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="O1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>
@@ -693,27 +693,27 @@
         <v>1959</v>
       </c>
       <c r="I2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L2" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="M2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>
@@ -734,27 +734,27 @@
         <v>1988</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="M3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>12</v>
@@ -775,27 +775,27 @@
         <v>1957</v>
       </c>
       <c r="I4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" t="s">
-        <v>42</v>
+        <v>31</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="L4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="M4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>16</v>
@@ -816,27 +816,27 @@
         <v>1991</v>
       </c>
       <c r="I5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J5" t="s">
-        <v>34</v>
-      </c>
-      <c r="K5" t="s">
-        <v>43</v>
+        <v>33</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="L5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="M5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
@@ -857,19 +857,19 @@
         <v>1958</v>
       </c>
       <c r="I6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J6" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" t="s">
-        <v>44</v>
+        <v>32</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="L6">
         <v>514</v>
       </c>
       <c r="M6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -879,6 +879,9 @@
     <hyperlink ref="D4" r:id="rId3" display="https://www.uade.edu.ar/" xr:uid="{A61D4A19-8C1C-5F41-8EC7-F17B85D4FF97}"/>
     <hyperlink ref="D5" r:id="rId4" display="https://www.utdt.edu/" xr:uid="{E544F7EF-372C-1544-8194-AD8651EFE0B3}"/>
     <hyperlink ref="D6" r:id="rId5" xr:uid="{EE27BF68-3AA7-024E-98BB-09C4C603D2D2}"/>
+    <hyperlink ref="K6" r:id="rId6" display="https://scontent.faep24-1.fna.fbcdn.net/v/t39.30808-6/327436997_1930120767319004_2025655574534719690_n.jpg?_nc_cat=106&amp;ccb=1-7&amp;_nc_sid=6ee11a&amp;_nc_ohc=ZT5iJ-GczfIQ7kNvgGLXHT7&amp;_nc_ht=scontent.faep24-1.fna&amp;oh=00_AYCs68elqgKBSAsJJ5NhhFSDiMgx3CzdCr7dlHREroTiag&amp;oe=668CB904" xr:uid="{A08C882B-E993-4FD3-AFFD-23351EAADE2C}"/>
+    <hyperlink ref="K5" r:id="rId7" xr:uid="{4E9780E0-D9C2-487E-A835-F8BF69EF150C}"/>
+    <hyperlink ref="K4" r:id="rId8" xr:uid="{21843420-A6BA-45B8-9F04-CAED497F4371}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>